<commit_message>
[Añadimos excel de eventos y creamos los mapas de pases, tiros y mapa de calor] Victor
</commit_message>
<xml_diff>
--- a/eventos.xlsx
+++ b/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Víctor\Desktop\IronHack\Apuntes\Futbol_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55867D5-DEB3-4032-8409-291612DADE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042F3E3D-54ED-47CA-959E-98BB7C766902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="144">
   <si>
     <t>timestamp</t>
   </si>
@@ -139,6 +139,324 @@
   </si>
   <si>
     <t>Raúl Angullo</t>
+  </si>
+  <si>
+    <t>00:00:07.782</t>
+  </si>
+  <si>
+    <t>00:00:08.242</t>
+  </si>
+  <si>
+    <t>Juan Camilo</t>
+  </si>
+  <si>
+    <t>00:00:08.970</t>
+  </si>
+  <si>
+    <t>Miscontrol</t>
+  </si>
+  <si>
+    <t>Clearance</t>
+  </si>
+  <si>
+    <t>00:00:09.762</t>
+  </si>
+  <si>
+    <t>Pablo Escribano</t>
+  </si>
+  <si>
+    <t>00:00:14.480</t>
+  </si>
+  <si>
+    <t>Duel</t>
+  </si>
+  <si>
+    <t>Alejandro Charro</t>
+  </si>
+  <si>
+    <t>Ball Recovery</t>
+  </si>
+  <si>
+    <t>00:00:19.040</t>
+  </si>
+  <si>
+    <t>Ramón Salas</t>
+  </si>
+  <si>
+    <t>00:00:20.520</t>
+  </si>
+  <si>
+    <t>Throw-in</t>
+  </si>
+  <si>
+    <t>00:00:31.370</t>
+  </si>
+  <si>
+    <t>Adrian Pombo</t>
+  </si>
+  <si>
+    <t>Fabio Patus</t>
+  </si>
+  <si>
+    <t>00:00:32.690</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>00:00:34.630</t>
+  </si>
+  <si>
+    <t>Daniel Serrano</t>
+  </si>
+  <si>
+    <t>00:00:36.230</t>
+  </si>
+  <si>
+    <t>Cesar Sanchez</t>
+  </si>
+  <si>
+    <t>00:00:45.210</t>
+  </si>
+  <si>
+    <t>00:00:47.210</t>
+  </si>
+  <si>
+    <t>00:00:49.210</t>
+  </si>
+  <si>
+    <t>Interception</t>
+  </si>
+  <si>
+    <t>00:00:48.470</t>
+  </si>
+  <si>
+    <t>00:00:52.220</t>
+  </si>
+  <si>
+    <t>00:01:06.540</t>
+  </si>
+  <si>
+    <t>Santiago Sanchez</t>
+  </si>
+  <si>
+    <t>00:01:08.040</t>
+  </si>
+  <si>
+    <t>00:01:09.080</t>
+  </si>
+  <si>
+    <t>Guillermo Escalera</t>
+  </si>
+  <si>
+    <t>00:01:09.580</t>
+  </si>
+  <si>
+    <t>00:01:10.890</t>
+  </si>
+  <si>
+    <t>00:01:14.890</t>
+  </si>
+  <si>
+    <t>Diego Refoyo</t>
+  </si>
+  <si>
+    <t>Foul Committed</t>
+  </si>
+  <si>
+    <t>00:01:25.890</t>
+  </si>
+  <si>
+    <t>00:01:27.120</t>
+  </si>
+  <si>
+    <t>00:01:26.760</t>
+  </si>
+  <si>
+    <t>00:01:29.580</t>
+  </si>
+  <si>
+    <t>00:01:32.580</t>
+  </si>
+  <si>
+    <t>00:01:34.330</t>
+  </si>
+  <si>
+    <t>00:01:36.690</t>
+  </si>
+  <si>
+    <t>00:01:38.090</t>
+  </si>
+  <si>
+    <t>Oscar López</t>
+  </si>
+  <si>
+    <t>00:01:39.020</t>
+  </si>
+  <si>
+    <t>00:01:39.620</t>
+  </si>
+  <si>
+    <t>00:01:42.020</t>
+  </si>
+  <si>
+    <t>Carlos Enrique</t>
+  </si>
+  <si>
+    <t>00:01:43.090</t>
+  </si>
+  <si>
+    <t>00:01:45.090</t>
+  </si>
+  <si>
+    <t>00:01:46.470</t>
+  </si>
+  <si>
+    <t>00:01:47.370</t>
+  </si>
+  <si>
+    <t>00:01:49.020</t>
+  </si>
+  <si>
+    <t>Dribble</t>
+  </si>
+  <si>
+    <t>00:01:49.920</t>
+  </si>
+  <si>
+    <t>Josue Serrano</t>
+  </si>
+  <si>
+    <t>00:01:50.200</t>
+  </si>
+  <si>
+    <t>00:01:51.600</t>
+  </si>
+  <si>
+    <t>00:01:52.120</t>
+  </si>
+  <si>
+    <t>00:01:54.120</t>
+  </si>
+  <si>
+    <t>00:01:55.120</t>
+  </si>
+  <si>
+    <t>Francisco José</t>
+  </si>
+  <si>
+    <t>00:01:57.800</t>
+  </si>
+  <si>
+    <t>00:01:58.030</t>
+  </si>
+  <si>
+    <t>00:01:59.590</t>
+  </si>
+  <si>
+    <t>00:02:00.710</t>
+  </si>
+  <si>
+    <t>Shot</t>
+  </si>
+  <si>
+    <t>Right Foot</t>
+  </si>
+  <si>
+    <t>Off T</t>
+  </si>
+  <si>
+    <t>Open Play</t>
+  </si>
+  <si>
+    <t>Goal Keeper</t>
+  </si>
+  <si>
+    <t>Ignacio Salas</t>
+  </si>
+  <si>
+    <t>00:02:02.710</t>
+  </si>
+  <si>
+    <t>00:02:33.090</t>
+  </si>
+  <si>
+    <t>00:02:38.090</t>
+  </si>
+  <si>
+    <t>00:02:38.240</t>
+  </si>
+  <si>
+    <t>00:02:40.240</t>
+  </si>
+  <si>
+    <t>00:02:42.240</t>
+  </si>
+  <si>
+    <t>00:03:07.240</t>
+  </si>
+  <si>
+    <t>00:03:10.240</t>
+  </si>
+  <si>
+    <t>Sebastian Olivares</t>
+  </si>
+  <si>
+    <t>00:03:11.040</t>
+  </si>
+  <si>
+    <t>00:03:12.340</t>
+  </si>
+  <si>
+    <t>Left Foot</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>00:03:56.340</t>
+  </si>
+  <si>
+    <t>00:03:58.340</t>
+  </si>
+  <si>
+    <t>00:04:00.340</t>
+  </si>
+  <si>
+    <t>00:03:59.340</t>
+  </si>
+  <si>
+    <t>00:04:02.340</t>
+  </si>
+  <si>
+    <t>00:04:03.740</t>
+  </si>
+  <si>
+    <t>00:04:08.330</t>
+  </si>
+  <si>
+    <t>00:04:23.330</t>
+  </si>
+  <si>
+    <t>00:04:25.330</t>
+  </si>
+  <si>
+    <t>00:04:28.330</t>
+  </si>
+  <si>
+    <t>00:04:35.330</t>
+  </si>
+  <si>
+    <t>00:04:30.330</t>
+  </si>
+  <si>
+    <t>00:04:38.330</t>
+  </si>
+  <si>
+    <t>00:04:37.730</t>
+  </si>
+  <si>
+    <t>00:04:39.000</t>
   </si>
 </sst>
 </file>
@@ -464,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="M83" sqref="M83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,6 +1085,2419 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>84</v>
+      </c>
+      <c r="F10">
+        <v>56</v>
+      </c>
+      <c r="L10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>84</v>
+      </c>
+      <c r="F11">
+        <v>56</v>
+      </c>
+      <c r="G11">
+        <v>94</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>94</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="L12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>98</v>
+      </c>
+      <c r="F13">
+        <v>36</v>
+      </c>
+      <c r="G13">
+        <v>48</v>
+      </c>
+      <c r="H13">
+        <v>55</v>
+      </c>
+      <c r="L13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <v>55</v>
+      </c>
+      <c r="L14" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>57</v>
+      </c>
+      <c r="L15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>68</v>
+      </c>
+      <c r="G16">
+        <v>27</v>
+      </c>
+      <c r="H16">
+        <v>80</v>
+      </c>
+      <c r="L16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>80</v>
+      </c>
+      <c r="M17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>27</v>
+      </c>
+      <c r="F18">
+        <v>80</v>
+      </c>
+      <c r="G18">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>65</v>
+      </c>
+      <c r="I18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>21</v>
+      </c>
+      <c r="F19">
+        <v>65</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>72</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>80</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>80</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>80</v>
+      </c>
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>62</v>
+      </c>
+      <c r="G23">
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>55</v>
+      </c>
+      <c r="I23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>55</v>
+      </c>
+      <c r="L24" t="s">
+        <v>51</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>58</v>
+      </c>
+      <c r="G25">
+        <v>42</v>
+      </c>
+      <c r="H25">
+        <v>80</v>
+      </c>
+      <c r="L25" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>42</v>
+      </c>
+      <c r="F26">
+        <v>80</v>
+      </c>
+      <c r="M26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>42</v>
+      </c>
+      <c r="F27">
+        <v>80</v>
+      </c>
+      <c r="G27">
+        <v>39</v>
+      </c>
+      <c r="H27">
+        <v>68</v>
+      </c>
+      <c r="I27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>39</v>
+      </c>
+      <c r="F28">
+        <v>68</v>
+      </c>
+      <c r="G28">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <v>62</v>
+      </c>
+      <c r="J28" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28" t="s">
+        <v>36</v>
+      </c>
+      <c r="L28" t="s">
+        <v>70</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <v>62</v>
+      </c>
+      <c r="L29" t="s">
+        <v>73</v>
+      </c>
+      <c r="M29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>64</v>
+      </c>
+      <c r="G30">
+        <v>42</v>
+      </c>
+      <c r="H30">
+        <v>68</v>
+      </c>
+      <c r="L30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>42</v>
+      </c>
+      <c r="F31">
+        <v>68</v>
+      </c>
+      <c r="L31" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>54</v>
+      </c>
+      <c r="F32">
+        <v>59</v>
+      </c>
+      <c r="L32" t="s">
+        <v>77</v>
+      </c>
+      <c r="M32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>54</v>
+      </c>
+      <c r="F33">
+        <v>59</v>
+      </c>
+      <c r="G33">
+        <v>50</v>
+      </c>
+      <c r="H33">
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>51</v>
+      </c>
+      <c r="J33" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" t="s">
+        <v>73</v>
+      </c>
+      <c r="M33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>50</v>
+      </c>
+      <c r="F34">
+        <v>66</v>
+      </c>
+      <c r="L34" t="s">
+        <v>51</v>
+      </c>
+      <c r="M34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>50</v>
+      </c>
+      <c r="F35">
+        <v>66</v>
+      </c>
+      <c r="G35">
+        <v>54</v>
+      </c>
+      <c r="H35">
+        <v>35</v>
+      </c>
+      <c r="I35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" t="s">
+        <v>51</v>
+      </c>
+      <c r="M35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>53</v>
+      </c>
+      <c r="F36">
+        <v>35</v>
+      </c>
+      <c r="L36" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>56</v>
+      </c>
+      <c r="F37">
+        <v>32</v>
+      </c>
+      <c r="G37">
+        <v>84</v>
+      </c>
+      <c r="H37">
+        <v>62</v>
+      </c>
+      <c r="I37" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>84</v>
+      </c>
+      <c r="F38">
+        <v>62</v>
+      </c>
+      <c r="G38">
+        <v>95</v>
+      </c>
+      <c r="H38">
+        <v>48</v>
+      </c>
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" t="s">
+        <v>33</v>
+      </c>
+      <c r="L38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>95</v>
+      </c>
+      <c r="F39">
+        <v>45</v>
+      </c>
+      <c r="G39">
+        <v>91</v>
+      </c>
+      <c r="H39">
+        <v>42</v>
+      </c>
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" t="s">
+        <v>36</v>
+      </c>
+      <c r="L39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>91</v>
+      </c>
+      <c r="F40">
+        <v>42</v>
+      </c>
+      <c r="L40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>91</v>
+      </c>
+      <c r="F41">
+        <v>42</v>
+      </c>
+      <c r="G41">
+        <v>89</v>
+      </c>
+      <c r="H41">
+        <v>38</v>
+      </c>
+      <c r="I41" t="s">
+        <v>87</v>
+      </c>
+      <c r="J41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" t="s">
+        <v>37</v>
+      </c>
+      <c r="M41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>89</v>
+      </c>
+      <c r="F42">
+        <v>38</v>
+      </c>
+      <c r="G42">
+        <v>102</v>
+      </c>
+      <c r="H42">
+        <v>18</v>
+      </c>
+      <c r="J42" t="s">
+        <v>58</v>
+      </c>
+      <c r="K42" t="s">
+        <v>36</v>
+      </c>
+      <c r="L42" t="s">
+        <v>87</v>
+      </c>
+      <c r="M42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>102</v>
+      </c>
+      <c r="F43">
+        <v>18</v>
+      </c>
+      <c r="L43" t="s">
+        <v>91</v>
+      </c>
+      <c r="M43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>102</v>
+      </c>
+      <c r="F44">
+        <v>18</v>
+      </c>
+      <c r="G44">
+        <v>65</v>
+      </c>
+      <c r="H44">
+        <v>22</v>
+      </c>
+      <c r="I44" t="s">
+        <v>48</v>
+      </c>
+      <c r="J44" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L44" t="s">
+        <v>91</v>
+      </c>
+      <c r="M44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>65</v>
+      </c>
+      <c r="F45">
+        <v>22</v>
+      </c>
+      <c r="L45" t="s">
+        <v>48</v>
+      </c>
+      <c r="M45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>65</v>
+      </c>
+      <c r="F46">
+        <v>22</v>
+      </c>
+      <c r="G46">
+        <v>72</v>
+      </c>
+      <c r="H46">
+        <v>18</v>
+      </c>
+      <c r="I46" t="s">
+        <v>70</v>
+      </c>
+      <c r="J46" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" t="s">
+        <v>48</v>
+      </c>
+      <c r="M46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>72</v>
+      </c>
+      <c r="F47">
+        <v>18</v>
+      </c>
+      <c r="L47" t="s">
+        <v>70</v>
+      </c>
+      <c r="M47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>69</v>
+      </c>
+      <c r="F48">
+        <v>20</v>
+      </c>
+      <c r="L48" t="s">
+        <v>70</v>
+      </c>
+      <c r="M48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>64</v>
+      </c>
+      <c r="F49">
+        <v>22</v>
+      </c>
+      <c r="G49">
+        <v>70</v>
+      </c>
+      <c r="H49">
+        <v>25</v>
+      </c>
+      <c r="I49" t="s">
+        <v>99</v>
+      </c>
+      <c r="J49" t="s">
+        <v>27</v>
+      </c>
+      <c r="K49" t="s">
+        <v>28</v>
+      </c>
+      <c r="L49" t="s">
+        <v>70</v>
+      </c>
+      <c r="M49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>70</v>
+      </c>
+      <c r="F50">
+        <v>25</v>
+      </c>
+      <c r="L50" t="s">
+        <v>99</v>
+      </c>
+      <c r="M50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>70</v>
+      </c>
+      <c r="F51">
+        <v>25</v>
+      </c>
+      <c r="G51">
+        <v>56</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51" t="s">
+        <v>70</v>
+      </c>
+      <c r="J51" t="s">
+        <v>27</v>
+      </c>
+      <c r="K51" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" t="s">
+        <v>99</v>
+      </c>
+      <c r="M51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>56</v>
+      </c>
+      <c r="F52">
+        <v>5</v>
+      </c>
+      <c r="L52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>53</v>
+      </c>
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <v>30</v>
+      </c>
+      <c r="H53">
+        <v>8</v>
+      </c>
+      <c r="J53" t="s">
+        <v>58</v>
+      </c>
+      <c r="K53" t="s">
+        <v>28</v>
+      </c>
+      <c r="L53" t="s">
+        <v>70</v>
+      </c>
+      <c r="M53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>18</v>
+      </c>
+      <c r="F54">
+        <v>15</v>
+      </c>
+      <c r="G54">
+        <v>37</v>
+      </c>
+      <c r="H54">
+        <v>15</v>
+      </c>
+      <c r="J54" t="s">
+        <v>58</v>
+      </c>
+      <c r="K54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54" t="s">
+        <v>105</v>
+      </c>
+      <c r="M54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>37</v>
+      </c>
+      <c r="F55">
+        <v>15</v>
+      </c>
+      <c r="L55" t="s">
+        <v>91</v>
+      </c>
+      <c r="M55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>37</v>
+      </c>
+      <c r="F56">
+        <v>15</v>
+      </c>
+      <c r="G56">
+        <v>16</v>
+      </c>
+      <c r="H56">
+        <v>20</v>
+      </c>
+      <c r="J56" t="s">
+        <v>58</v>
+      </c>
+      <c r="K56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" t="s">
+        <v>91</v>
+      </c>
+      <c r="M56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>16</v>
+      </c>
+      <c r="F57">
+        <v>20</v>
+      </c>
+      <c r="L57" t="s">
+        <v>25</v>
+      </c>
+      <c r="M57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>19</v>
+      </c>
+      <c r="F58">
+        <v>31</v>
+      </c>
+      <c r="L58" t="s">
+        <v>99</v>
+      </c>
+      <c r="M58" t="s">
+        <v>15</v>
+      </c>
+      <c r="O58" t="s">
+        <v>111</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>36</v>
+      </c>
+      <c r="R58">
+        <v>120</v>
+      </c>
+      <c r="S58" t="s">
+        <v>112</v>
+      </c>
+      <c r="T58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="L59" t="s">
+        <v>115</v>
+      </c>
+      <c r="M59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>7</v>
+      </c>
+      <c r="F60">
+        <v>40</v>
+      </c>
+      <c r="G60">
+        <v>60</v>
+      </c>
+      <c r="H60">
+        <v>62</v>
+      </c>
+      <c r="J60" t="s">
+        <v>58</v>
+      </c>
+      <c r="K60" t="s">
+        <v>33</v>
+      </c>
+      <c r="L60" t="s">
+        <v>115</v>
+      </c>
+      <c r="M60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>60</v>
+      </c>
+      <c r="F61">
+        <v>57</v>
+      </c>
+      <c r="L61" t="s">
+        <v>37</v>
+      </c>
+      <c r="M61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>60</v>
+      </c>
+      <c r="F62">
+        <v>57</v>
+      </c>
+      <c r="G62">
+        <v>75</v>
+      </c>
+      <c r="H62">
+        <v>57</v>
+      </c>
+      <c r="I62" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" t="s">
+        <v>33</v>
+      </c>
+      <c r="L62" t="s">
+        <v>37</v>
+      </c>
+      <c r="M62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>75</v>
+      </c>
+      <c r="F63">
+        <v>57</v>
+      </c>
+      <c r="L63" t="s">
+        <v>26</v>
+      </c>
+      <c r="M63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>85</v>
+      </c>
+      <c r="F64">
+        <v>50</v>
+      </c>
+      <c r="L64" t="s">
+        <v>40</v>
+      </c>
+      <c r="M64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>85</v>
+      </c>
+      <c r="F65">
+        <v>50</v>
+      </c>
+      <c r="G65">
+        <v>108</v>
+      </c>
+      <c r="H65">
+        <v>35</v>
+      </c>
+      <c r="J65" t="s">
+        <v>58</v>
+      </c>
+      <c r="K65" t="s">
+        <v>33</v>
+      </c>
+      <c r="L65" t="s">
+        <v>87</v>
+      </c>
+      <c r="M65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>106</v>
+      </c>
+      <c r="F66">
+        <v>32</v>
+      </c>
+      <c r="L66" t="s">
+        <v>124</v>
+      </c>
+      <c r="M66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>106</v>
+      </c>
+      <c r="F67">
+        <v>32</v>
+      </c>
+      <c r="G67">
+        <v>102</v>
+      </c>
+      <c r="H67">
+        <v>40</v>
+      </c>
+      <c r="I67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J67" t="s">
+        <v>27</v>
+      </c>
+      <c r="K67" t="s">
+        <v>28</v>
+      </c>
+      <c r="L67" t="s">
+        <v>124</v>
+      </c>
+      <c r="M67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>102</v>
+      </c>
+      <c r="F68">
+        <v>40</v>
+      </c>
+      <c r="L68" t="s">
+        <v>37</v>
+      </c>
+      <c r="M68" t="s">
+        <v>14</v>
+      </c>
+      <c r="O68" t="s">
+        <v>127</v>
+      </c>
+      <c r="P68">
+        <v>120</v>
+      </c>
+      <c r="Q68">
+        <v>37</v>
+      </c>
+      <c r="R68">
+        <v>3</v>
+      </c>
+      <c r="S68" t="s">
+        <v>128</v>
+      </c>
+      <c r="T68" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <v>60</v>
+      </c>
+      <c r="F69">
+        <v>40</v>
+      </c>
+      <c r="G69">
+        <v>81</v>
+      </c>
+      <c r="H69">
+        <v>40</v>
+      </c>
+      <c r="J69" t="s">
+        <v>27</v>
+      </c>
+      <c r="K69" t="s">
+        <v>28</v>
+      </c>
+      <c r="L69" t="s">
+        <v>48</v>
+      </c>
+      <c r="M69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70">
+        <v>81</v>
+      </c>
+      <c r="F70">
+        <v>40</v>
+      </c>
+      <c r="L70" t="s">
+        <v>77</v>
+      </c>
+      <c r="M70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>81</v>
+      </c>
+      <c r="F71">
+        <v>40</v>
+      </c>
+      <c r="G71">
+        <v>86</v>
+      </c>
+      <c r="H71">
+        <v>18</v>
+      </c>
+      <c r="I71" t="s">
+        <v>91</v>
+      </c>
+      <c r="J71" t="s">
+        <v>27</v>
+      </c>
+      <c r="K71" t="s">
+        <v>28</v>
+      </c>
+      <c r="L71" t="s">
+        <v>77</v>
+      </c>
+      <c r="M71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72">
+        <v>4</v>
+      </c>
+      <c r="E72">
+        <v>86</v>
+      </c>
+      <c r="F72">
+        <v>18</v>
+      </c>
+      <c r="L72" t="s">
+        <v>91</v>
+      </c>
+      <c r="M72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+      <c r="E73">
+        <v>84</v>
+      </c>
+      <c r="F73">
+        <v>18</v>
+      </c>
+      <c r="G73">
+        <v>41</v>
+      </c>
+      <c r="H73">
+        <v>22</v>
+      </c>
+      <c r="I73" t="s">
+        <v>48</v>
+      </c>
+      <c r="J73" t="s">
+        <v>27</v>
+      </c>
+      <c r="K73" t="s">
+        <v>33</v>
+      </c>
+      <c r="L73" t="s">
+        <v>91</v>
+      </c>
+      <c r="M73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <v>41</v>
+      </c>
+      <c r="F74">
+        <v>22</v>
+      </c>
+      <c r="L74" t="s">
+        <v>48</v>
+      </c>
+      <c r="M74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+      <c r="L75" t="s">
+        <v>115</v>
+      </c>
+      <c r="M75" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>7</v>
+      </c>
+      <c r="F76">
+        <v>33</v>
+      </c>
+      <c r="G76">
+        <v>9</v>
+      </c>
+      <c r="H76">
+        <v>20</v>
+      </c>
+      <c r="I76" t="s">
+        <v>25</v>
+      </c>
+      <c r="J76" t="s">
+        <v>27</v>
+      </c>
+      <c r="K76" t="s">
+        <v>28</v>
+      </c>
+      <c r="L76" t="s">
+        <v>115</v>
+      </c>
+      <c r="M76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77">
+        <v>4</v>
+      </c>
+      <c r="E77">
+        <v>9</v>
+      </c>
+      <c r="F77">
+        <v>20</v>
+      </c>
+      <c r="L77" t="s">
+        <v>25</v>
+      </c>
+      <c r="M77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78">
+        <v>18</v>
+      </c>
+      <c r="F78">
+        <v>18</v>
+      </c>
+      <c r="G78">
+        <v>72</v>
+      </c>
+      <c r="H78">
+        <v>19</v>
+      </c>
+      <c r="J78" t="s">
+        <v>58</v>
+      </c>
+      <c r="K78" t="s">
+        <v>33</v>
+      </c>
+      <c r="L78" t="s">
+        <v>25</v>
+      </c>
+      <c r="M78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" t="s">
+        <v>43</v>
+      </c>
+      <c r="D79">
+        <v>4</v>
+      </c>
+      <c r="E79">
+        <v>72</v>
+      </c>
+      <c r="F79">
+        <v>19</v>
+      </c>
+      <c r="G79">
+        <v>67</v>
+      </c>
+      <c r="H79">
+        <v>23</v>
+      </c>
+      <c r="L79" t="s">
+        <v>70</v>
+      </c>
+      <c r="M79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80">
+        <v>71</v>
+      </c>
+      <c r="F80">
+        <v>32</v>
+      </c>
+      <c r="L80" t="s">
+        <v>26</v>
+      </c>
+      <c r="M80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>142</v>
+      </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" t="s">
+        <v>49</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81">
+        <v>69</v>
+      </c>
+      <c r="F81">
+        <v>27</v>
+      </c>
+      <c r="L81" t="s">
+        <v>77</v>
+      </c>
+      <c r="M81" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82">
+        <v>4</v>
+      </c>
+      <c r="E82">
+        <v>69</v>
+      </c>
+      <c r="F82">
+        <v>27</v>
+      </c>
+      <c r="G82">
+        <v>80</v>
+      </c>
+      <c r="H82">
+        <v>54</v>
+      </c>
+      <c r="I82" t="s">
+        <v>70</v>
+      </c>
+      <c r="J82" t="s">
+        <v>27</v>
+      </c>
+      <c r="K82" t="s">
+        <v>28</v>
+      </c>
+      <c r="L82" t="s">
+        <v>77</v>
+      </c>
+      <c r="M82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>143</v>
+      </c>
+      <c r="B83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83">
+        <v>80</v>
+      </c>
+      <c r="F83">
+        <v>54</v>
+      </c>
+      <c r="L83" t="s">
+        <v>70</v>
+      </c>
+      <c r="M83" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
[Añadimos a StreamLit la pantalla de gráficos de analisis de partidos] Victor
</commit_message>
<xml_diff>
--- a/eventos.xlsx
+++ b/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Víctor\Desktop\IronHack\Apuntes\Futbol_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042F3E3D-54ED-47CA-959E-98BB7C766902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F586935-2608-46BB-95D1-2107C6E1E0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="173">
   <si>
     <t>timestamp</t>
   </si>
@@ -457,6 +457,93 @@
   </si>
   <si>
     <t>00:04:39.000</t>
+  </si>
+  <si>
+    <t>00:04:43.530</t>
+  </si>
+  <si>
+    <t>00:04:45.950</t>
+  </si>
+  <si>
+    <t>00:04:46.850</t>
+  </si>
+  <si>
+    <t>00:04:48.350</t>
+  </si>
+  <si>
+    <t>00:04:49.850</t>
+  </si>
+  <si>
+    <t>00:05:09.250</t>
+  </si>
+  <si>
+    <t>00:05:12.250</t>
+  </si>
+  <si>
+    <t>00:05:14.250</t>
+  </si>
+  <si>
+    <t>00:05:15.290</t>
+  </si>
+  <si>
+    <t>00:05:17.290</t>
+  </si>
+  <si>
+    <t>Misdribble</t>
+  </si>
+  <si>
+    <t>00:05:19.800</t>
+  </si>
+  <si>
+    <t>00:05:20.800</t>
+  </si>
+  <si>
+    <t>Ángel Jesús</t>
+  </si>
+  <si>
+    <t>00:05:33.700</t>
+  </si>
+  <si>
+    <t>Oscar Ponce</t>
+  </si>
+  <si>
+    <t>00:05:35.940</t>
+  </si>
+  <si>
+    <t>00:05:37.110</t>
+  </si>
+  <si>
+    <t>00:05:38.680</t>
+  </si>
+  <si>
+    <t>00:05:40.680</t>
+  </si>
+  <si>
+    <t>00:05:42.680</t>
+  </si>
+  <si>
+    <t>00:05:43.680</t>
+  </si>
+  <si>
+    <t>00:05:45.400</t>
+  </si>
+  <si>
+    <t>00:05:46.630</t>
+  </si>
+  <si>
+    <t>00:05:49.640</t>
+  </si>
+  <si>
+    <t>00:05:51.640</t>
+  </si>
+  <si>
+    <t>00:05:53.640</t>
+  </si>
+  <si>
+    <t>00:05:55.310</t>
+  </si>
+  <si>
+    <t>00:05:56.510</t>
   </si>
 </sst>
 </file>
@@ -782,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="M83" sqref="M83"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="Q101" sqref="Q101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3498,6 +3585,844 @@
         <v>15</v>
       </c>
     </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>144</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" t="s">
+        <v>32</v>
+      </c>
+      <c r="D84">
+        <v>4</v>
+      </c>
+      <c r="E84">
+        <v>50</v>
+      </c>
+      <c r="F84">
+        <v>60</v>
+      </c>
+      <c r="G84">
+        <v>33</v>
+      </c>
+      <c r="H84">
+        <v>74</v>
+      </c>
+      <c r="I84" t="s">
+        <v>55</v>
+      </c>
+      <c r="J84" t="s">
+        <v>27</v>
+      </c>
+      <c r="K84" t="s">
+        <v>28</v>
+      </c>
+      <c r="L84" t="s">
+        <v>70</v>
+      </c>
+      <c r="M84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <v>33</v>
+      </c>
+      <c r="F85">
+        <v>74</v>
+      </c>
+      <c r="L85" t="s">
+        <v>55</v>
+      </c>
+      <c r="M85" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" t="s">
+        <v>32</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86">
+        <v>30</v>
+      </c>
+      <c r="F86">
+        <v>74</v>
+      </c>
+      <c r="G86">
+        <v>15</v>
+      </c>
+      <c r="H86">
+        <v>50</v>
+      </c>
+      <c r="I86" t="s">
+        <v>48</v>
+      </c>
+      <c r="J86" t="s">
+        <v>27</v>
+      </c>
+      <c r="K86" t="s">
+        <v>33</v>
+      </c>
+      <c r="L86" t="s">
+        <v>55</v>
+      </c>
+      <c r="M86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87">
+        <v>15</v>
+      </c>
+      <c r="F87">
+        <v>50</v>
+      </c>
+      <c r="L87" t="s">
+        <v>48</v>
+      </c>
+      <c r="M87" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>148</v>
+      </c>
+      <c r="B88" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88">
+        <v>4</v>
+      </c>
+      <c r="F88">
+        <v>47</v>
+      </c>
+      <c r="L88" t="s">
+        <v>115</v>
+      </c>
+      <c r="M88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>149</v>
+      </c>
+      <c r="B89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" t="s">
+        <v>32</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="E89">
+        <v>21</v>
+      </c>
+      <c r="F89">
+        <v>42</v>
+      </c>
+      <c r="G89">
+        <v>81</v>
+      </c>
+      <c r="H89">
+        <v>60</v>
+      </c>
+      <c r="J89" t="s">
+        <v>58</v>
+      </c>
+      <c r="K89" t="s">
+        <v>33</v>
+      </c>
+      <c r="L89" t="s">
+        <v>115</v>
+      </c>
+      <c r="M89" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>150</v>
+      </c>
+      <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+      <c r="E90">
+        <v>81</v>
+      </c>
+      <c r="F90">
+        <v>60</v>
+      </c>
+      <c r="L90" t="s">
+        <v>55</v>
+      </c>
+      <c r="M90" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>151</v>
+      </c>
+      <c r="B91" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+      <c r="E91">
+        <v>83</v>
+      </c>
+      <c r="F91">
+        <v>58</v>
+      </c>
+      <c r="L91" t="s">
+        <v>40</v>
+      </c>
+      <c r="M91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>152</v>
+      </c>
+      <c r="B92" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <v>83</v>
+      </c>
+      <c r="F92">
+        <v>58</v>
+      </c>
+      <c r="G92">
+        <v>102</v>
+      </c>
+      <c r="H92">
+        <v>62</v>
+      </c>
+      <c r="I92" t="s">
+        <v>37</v>
+      </c>
+      <c r="J92" t="s">
+        <v>27</v>
+      </c>
+      <c r="K92" t="s">
+        <v>33</v>
+      </c>
+      <c r="L92" t="s">
+        <v>40</v>
+      </c>
+      <c r="M92" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93">
+        <v>5</v>
+      </c>
+      <c r="E93">
+        <v>106</v>
+      </c>
+      <c r="F93">
+        <v>63</v>
+      </c>
+      <c r="L93" t="s">
+        <v>37</v>
+      </c>
+      <c r="M93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>155</v>
+      </c>
+      <c r="B94" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" t="s">
+        <v>154</v>
+      </c>
+      <c r="D94">
+        <v>5</v>
+      </c>
+      <c r="E94">
+        <v>108</v>
+      </c>
+      <c r="F94">
+        <v>65</v>
+      </c>
+      <c r="L94" t="s">
+        <v>37</v>
+      </c>
+      <c r="M94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>156</v>
+      </c>
+      <c r="B95" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" t="s">
+        <v>78</v>
+      </c>
+      <c r="D95">
+        <v>5</v>
+      </c>
+      <c r="E95">
+        <v>108</v>
+      </c>
+      <c r="F95">
+        <v>65</v>
+      </c>
+      <c r="L95" t="s">
+        <v>37</v>
+      </c>
+      <c r="M95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>158</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
+      <c r="E96">
+        <v>108</v>
+      </c>
+      <c r="F96">
+        <v>65</v>
+      </c>
+      <c r="G96">
+        <v>114</v>
+      </c>
+      <c r="H96">
+        <v>49</v>
+      </c>
+      <c r="I96" t="s">
+        <v>159</v>
+      </c>
+      <c r="J96" t="s">
+        <v>27</v>
+      </c>
+      <c r="K96" t="s">
+        <v>28</v>
+      </c>
+      <c r="L96" t="s">
+        <v>157</v>
+      </c>
+      <c r="M96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>160</v>
+      </c>
+      <c r="B97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97">
+        <v>5</v>
+      </c>
+      <c r="E97">
+        <v>114</v>
+      </c>
+      <c r="F97">
+        <v>49</v>
+      </c>
+      <c r="L97" t="s">
+        <v>159</v>
+      </c>
+      <c r="M97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" t="s">
+        <v>32</v>
+      </c>
+      <c r="D98">
+        <v>5</v>
+      </c>
+      <c r="E98">
+        <v>114</v>
+      </c>
+      <c r="F98">
+        <v>46</v>
+      </c>
+      <c r="G98">
+        <v>112</v>
+      </c>
+      <c r="H98">
+        <v>22</v>
+      </c>
+      <c r="I98" t="s">
+        <v>45</v>
+      </c>
+      <c r="J98" t="s">
+        <v>27</v>
+      </c>
+      <c r="K98" t="s">
+        <v>28</v>
+      </c>
+      <c r="L98" t="s">
+        <v>159</v>
+      </c>
+      <c r="M98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>162</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99">
+        <v>5</v>
+      </c>
+      <c r="E99">
+        <v>112</v>
+      </c>
+      <c r="F99">
+        <v>22</v>
+      </c>
+      <c r="L99" t="s">
+        <v>45</v>
+      </c>
+      <c r="M99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>163</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100">
+        <v>5</v>
+      </c>
+      <c r="E100">
+        <v>112</v>
+      </c>
+      <c r="F100">
+        <v>22</v>
+      </c>
+      <c r="G100">
+        <v>95</v>
+      </c>
+      <c r="H100">
+        <v>2</v>
+      </c>
+      <c r="I100" t="s">
+        <v>91</v>
+      </c>
+      <c r="J100" t="s">
+        <v>27</v>
+      </c>
+      <c r="K100" t="s">
+        <v>28</v>
+      </c>
+      <c r="L100" t="s">
+        <v>45</v>
+      </c>
+      <c r="M100" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>164</v>
+      </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101">
+        <v>5</v>
+      </c>
+      <c r="E101">
+        <v>95</v>
+      </c>
+      <c r="F101">
+        <v>2</v>
+      </c>
+      <c r="L101" t="s">
+        <v>91</v>
+      </c>
+      <c r="M101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102">
+        <v>5</v>
+      </c>
+      <c r="E102">
+        <v>95</v>
+      </c>
+      <c r="F102">
+        <v>2</v>
+      </c>
+      <c r="G102">
+        <v>102</v>
+      </c>
+      <c r="H102">
+        <v>24</v>
+      </c>
+      <c r="I102" t="s">
+        <v>45</v>
+      </c>
+      <c r="J102" t="s">
+        <v>27</v>
+      </c>
+      <c r="K102" t="s">
+        <v>28</v>
+      </c>
+      <c r="L102" t="s">
+        <v>91</v>
+      </c>
+      <c r="M102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103">
+        <v>5</v>
+      </c>
+      <c r="E103">
+        <v>102</v>
+      </c>
+      <c r="F103">
+        <v>24</v>
+      </c>
+      <c r="L103" t="s">
+        <v>45</v>
+      </c>
+      <c r="M103" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104">
+        <v>5</v>
+      </c>
+      <c r="E104">
+        <v>102</v>
+      </c>
+      <c r="F104">
+        <v>24</v>
+      </c>
+      <c r="G104">
+        <v>100</v>
+      </c>
+      <c r="H104">
+        <v>64</v>
+      </c>
+      <c r="I104" t="s">
+        <v>157</v>
+      </c>
+      <c r="J104" t="s">
+        <v>27</v>
+      </c>
+      <c r="K104" t="s">
+        <v>28</v>
+      </c>
+      <c r="L104" t="s">
+        <v>45</v>
+      </c>
+      <c r="M104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105">
+        <v>5</v>
+      </c>
+      <c r="E105">
+        <v>100</v>
+      </c>
+      <c r="F105">
+        <v>64</v>
+      </c>
+      <c r="L105" t="s">
+        <v>157</v>
+      </c>
+      <c r="M105" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" t="s">
+        <v>32</v>
+      </c>
+      <c r="D106">
+        <v>5</v>
+      </c>
+      <c r="E106">
+        <v>90</v>
+      </c>
+      <c r="F106">
+        <v>65</v>
+      </c>
+      <c r="G106">
+        <v>80</v>
+      </c>
+      <c r="H106">
+        <v>79</v>
+      </c>
+      <c r="I106" t="s">
+        <v>55</v>
+      </c>
+      <c r="J106" t="s">
+        <v>27</v>
+      </c>
+      <c r="K106" t="s">
+        <v>28</v>
+      </c>
+      <c r="L106" t="s">
+        <v>157</v>
+      </c>
+      <c r="M106" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>80</v>
+      </c>
+      <c r="F107">
+        <v>79</v>
+      </c>
+      <c r="L107" t="s">
+        <v>55</v>
+      </c>
+      <c r="M107" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" t="s">
+        <v>15</v>
+      </c>
+      <c r="C108" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108">
+        <v>5</v>
+      </c>
+      <c r="E108">
+        <v>80</v>
+      </c>
+      <c r="F108">
+        <v>76</v>
+      </c>
+      <c r="G108">
+        <v>86</v>
+      </c>
+      <c r="H108">
+        <v>77</v>
+      </c>
+      <c r="I108" t="s">
+        <v>157</v>
+      </c>
+      <c r="J108" t="s">
+        <v>27</v>
+      </c>
+      <c r="K108" t="s">
+        <v>28</v>
+      </c>
+      <c r="L108" t="s">
+        <v>55</v>
+      </c>
+      <c r="M108" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109" t="s">
+        <v>29</v>
+      </c>
+      <c r="D109">
+        <v>5</v>
+      </c>
+      <c r="E109">
+        <v>86</v>
+      </c>
+      <c r="F109">
+        <v>77</v>
+      </c>
+      <c r="L109" t="s">
+        <v>157</v>
+      </c>
+      <c r="M109" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
[Actualizamos predicciones para la Jornada 21] Victor
</commit_message>
<xml_diff>
--- a/eventos.xlsx
+++ b/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Víctor\Desktop\IronHack\Apuntes\Futbol_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F586935-2608-46BB-95D1-2107C6E1E0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE067536-40C5-4390-B8D4-598046C9413D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="236">
   <si>
     <t>timestamp</t>
   </si>
@@ -544,6 +544,195 @@
   </si>
   <si>
     <t>00:05:56.510</t>
+  </si>
+  <si>
+    <t>00:05:58.510</t>
+  </si>
+  <si>
+    <t>00:06:00.530</t>
+  </si>
+  <si>
+    <t>00:06:02.730</t>
+  </si>
+  <si>
+    <t>00:06:04.710</t>
+  </si>
+  <si>
+    <t>00:06:06.410</t>
+  </si>
+  <si>
+    <t>00:06:09.640</t>
+  </si>
+  <si>
+    <t>00:06:12.000</t>
+  </si>
+  <si>
+    <t>00:06:12.940</t>
+  </si>
+  <si>
+    <t>00:06:14.640</t>
+  </si>
+  <si>
+    <t>00:06:17.710</t>
+  </si>
+  <si>
+    <t>00:06:19.110</t>
+  </si>
+  <si>
+    <t>00:06:20.490</t>
+  </si>
+  <si>
+    <t>00:06:22.490</t>
+  </si>
+  <si>
+    <t>00:06:24.490</t>
+  </si>
+  <si>
+    <t>00:06:28.490</t>
+  </si>
+  <si>
+    <t>00:06:30.490</t>
+  </si>
+  <si>
+    <t>00:06:32.490</t>
+  </si>
+  <si>
+    <t>00:06:34.490</t>
+  </si>
+  <si>
+    <t>00:06:36.490</t>
+  </si>
+  <si>
+    <t>00:06:38.490</t>
+  </si>
+  <si>
+    <t>00:06:41.490</t>
+  </si>
+  <si>
+    <t>00:06:42.790</t>
+  </si>
+  <si>
+    <t>00:06:44.320</t>
+  </si>
+  <si>
+    <t>00:06:46.320</t>
+  </si>
+  <si>
+    <t>00:06:50.320</t>
+  </si>
+  <si>
+    <t>00:06:52.720</t>
+  </si>
+  <si>
+    <t>00:07:08.720</t>
+  </si>
+  <si>
+    <t>00:07:10.720</t>
+  </si>
+  <si>
+    <t>00:07:11.820</t>
+  </si>
+  <si>
+    <t>00:07:12.910</t>
+  </si>
+  <si>
+    <t>00:07:14.900</t>
+  </si>
+  <si>
+    <t>00:07:15.940</t>
+  </si>
+  <si>
+    <t>00:07:20.040</t>
+  </si>
+  <si>
+    <t>00:07:22.040</t>
+  </si>
+  <si>
+    <t>00:07:25.540</t>
+  </si>
+  <si>
+    <t>00:07:27.540</t>
+  </si>
+  <si>
+    <t>00:07:28.430</t>
+  </si>
+  <si>
+    <t>00:07:34.930</t>
+  </si>
+  <si>
+    <t>00:07:39.080</t>
+  </si>
+  <si>
+    <t>00:07:42.880</t>
+  </si>
+  <si>
+    <t>00:07:43.310</t>
+  </si>
+  <si>
+    <t>00:07:45.410</t>
+  </si>
+  <si>
+    <t>00:07:46.320</t>
+  </si>
+  <si>
+    <t>00:07:47.620</t>
+  </si>
+  <si>
+    <t>00:07:48.520</t>
+  </si>
+  <si>
+    <t>00:07:49.320</t>
+  </si>
+  <si>
+    <t>00:07:50.320</t>
+  </si>
+  <si>
+    <t>00:08:05.320</t>
+  </si>
+  <si>
+    <t>00:08:06.320</t>
+  </si>
+  <si>
+    <t>00:08:09.320</t>
+  </si>
+  <si>
+    <t>00:08:11.320</t>
+  </si>
+  <si>
+    <t>00:08:13.320</t>
+  </si>
+  <si>
+    <t>00:08:12.320</t>
+  </si>
+  <si>
+    <t>00:08:17.320</t>
+  </si>
+  <si>
+    <t>00:08:20.320</t>
+  </si>
+  <si>
+    <t>00:08:22.320</t>
+  </si>
+  <si>
+    <t>00:08:24.320</t>
+  </si>
+  <si>
+    <t>00:08:26.320</t>
+  </si>
+  <si>
+    <t>00:08:28.320</t>
+  </si>
+  <si>
+    <t>00:08:32.320</t>
+  </si>
+  <si>
+    <t>00:08:33.820</t>
+  </si>
+  <si>
+    <t>00:08:35.820</t>
+  </si>
+  <si>
+    <t>00:08:37.820</t>
   </si>
 </sst>
 </file>
@@ -586,9 +775,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T109"/>
+  <dimension ref="A1:T172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="Q101" sqref="Q101"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4423,6 +4613,2130 @@
         <v>15</v>
       </c>
     </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" t="s">
+        <v>97</v>
+      </c>
+      <c r="D110">
+        <v>5</v>
+      </c>
+      <c r="E110">
+        <v>86</v>
+      </c>
+      <c r="F110">
+        <v>77</v>
+      </c>
+      <c r="L110" t="s">
+        <v>157</v>
+      </c>
+      <c r="M110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" t="s">
+        <v>32</v>
+      </c>
+      <c r="D111">
+        <v>6</v>
+      </c>
+      <c r="E111">
+        <v>82</v>
+      </c>
+      <c r="F111">
+        <v>64</v>
+      </c>
+      <c r="G111">
+        <v>102</v>
+      </c>
+      <c r="H111">
+        <v>55</v>
+      </c>
+      <c r="I111" t="s">
+        <v>159</v>
+      </c>
+      <c r="J111" t="s">
+        <v>27</v>
+      </c>
+      <c r="K111" t="s">
+        <v>28</v>
+      </c>
+      <c r="L111" t="s">
+        <v>157</v>
+      </c>
+      <c r="M111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112">
+        <v>6</v>
+      </c>
+      <c r="E112">
+        <v>102</v>
+      </c>
+      <c r="F112">
+        <v>55</v>
+      </c>
+      <c r="L112" t="s">
+        <v>159</v>
+      </c>
+      <c r="M112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" t="s">
+        <v>32</v>
+      </c>
+      <c r="D113">
+        <v>6</v>
+      </c>
+      <c r="E113">
+        <v>104</v>
+      </c>
+      <c r="F113">
+        <v>46</v>
+      </c>
+      <c r="G113">
+        <v>91</v>
+      </c>
+      <c r="H113">
+        <v>6</v>
+      </c>
+      <c r="I113" t="s">
+        <v>91</v>
+      </c>
+      <c r="J113" t="s">
+        <v>27</v>
+      </c>
+      <c r="K113" t="s">
+        <v>28</v>
+      </c>
+      <c r="L113" t="s">
+        <v>159</v>
+      </c>
+      <c r="M113" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" t="s">
+        <v>29</v>
+      </c>
+      <c r="D114">
+        <v>6</v>
+      </c>
+      <c r="E114">
+        <v>91</v>
+      </c>
+      <c r="F114">
+        <v>6</v>
+      </c>
+      <c r="L114" t="s">
+        <v>91</v>
+      </c>
+      <c r="M114" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" t="s">
+        <v>32</v>
+      </c>
+      <c r="D115">
+        <v>6</v>
+      </c>
+      <c r="E115">
+        <v>80</v>
+      </c>
+      <c r="F115">
+        <v>6</v>
+      </c>
+      <c r="G115">
+        <v>59</v>
+      </c>
+      <c r="H115">
+        <v>20</v>
+      </c>
+      <c r="I115" t="s">
+        <v>70</v>
+      </c>
+      <c r="J115" t="s">
+        <v>27</v>
+      </c>
+      <c r="K115" t="s">
+        <v>28</v>
+      </c>
+      <c r="L115" t="s">
+        <v>91</v>
+      </c>
+      <c r="M115" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>179</v>
+      </c>
+      <c r="B116" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" t="s">
+        <v>29</v>
+      </c>
+      <c r="D116">
+        <v>6</v>
+      </c>
+      <c r="E116">
+        <v>59</v>
+      </c>
+      <c r="F116">
+        <v>20</v>
+      </c>
+      <c r="L116" t="s">
+        <v>70</v>
+      </c>
+      <c r="M116" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>180</v>
+      </c>
+      <c r="B117" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" t="s">
+        <v>32</v>
+      </c>
+      <c r="D117">
+        <v>6</v>
+      </c>
+      <c r="E117">
+        <v>59</v>
+      </c>
+      <c r="F117">
+        <v>20</v>
+      </c>
+      <c r="G117">
+        <v>55</v>
+      </c>
+      <c r="H117">
+        <v>2</v>
+      </c>
+      <c r="J117" t="s">
+        <v>58</v>
+      </c>
+      <c r="K117" t="s">
+        <v>28</v>
+      </c>
+      <c r="L117" t="s">
+        <v>70</v>
+      </c>
+      <c r="M117" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>181</v>
+      </c>
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>43</v>
+      </c>
+      <c r="D118">
+        <v>6</v>
+      </c>
+      <c r="E118">
+        <v>55</v>
+      </c>
+      <c r="F118">
+        <v>2</v>
+      </c>
+      <c r="G118">
+        <v>77</v>
+      </c>
+      <c r="H118">
+        <v>3</v>
+      </c>
+      <c r="L118" t="s">
+        <v>124</v>
+      </c>
+      <c r="M118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>182</v>
+      </c>
+      <c r="B119" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" t="s">
+        <v>29</v>
+      </c>
+      <c r="D119">
+        <v>6</v>
+      </c>
+      <c r="E119">
+        <v>77</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+      <c r="L119" t="s">
+        <v>45</v>
+      </c>
+      <c r="M119" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>183</v>
+      </c>
+      <c r="B120" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" t="s">
+        <v>32</v>
+      </c>
+      <c r="D120">
+        <v>6</v>
+      </c>
+      <c r="E120">
+        <v>77</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+      <c r="G120">
+        <v>104</v>
+      </c>
+      <c r="H120">
+        <v>36</v>
+      </c>
+      <c r="I120" t="s">
+        <v>159</v>
+      </c>
+      <c r="J120" t="s">
+        <v>27</v>
+      </c>
+      <c r="K120" t="s">
+        <v>28</v>
+      </c>
+      <c r="L120" t="s">
+        <v>45</v>
+      </c>
+      <c r="M120" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>184</v>
+      </c>
+      <c r="B121" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121">
+        <v>6</v>
+      </c>
+      <c r="E121">
+        <v>104</v>
+      </c>
+      <c r="F121">
+        <v>36</v>
+      </c>
+      <c r="L121" t="s">
+        <v>159</v>
+      </c>
+      <c r="M121" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>185</v>
+      </c>
+      <c r="B122" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" t="s">
+        <v>32</v>
+      </c>
+      <c r="D122">
+        <v>6</v>
+      </c>
+      <c r="E122">
+        <v>97</v>
+      </c>
+      <c r="F122">
+        <v>39</v>
+      </c>
+      <c r="G122">
+        <v>90</v>
+      </c>
+      <c r="H122">
+        <v>62</v>
+      </c>
+      <c r="I122" t="s">
+        <v>157</v>
+      </c>
+      <c r="J122" t="s">
+        <v>27</v>
+      </c>
+      <c r="K122" t="s">
+        <v>28</v>
+      </c>
+      <c r="L122" t="s">
+        <v>159</v>
+      </c>
+      <c r="M122" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>186</v>
+      </c>
+      <c r="B123" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" t="s">
+        <v>29</v>
+      </c>
+      <c r="D123">
+        <v>6</v>
+      </c>
+      <c r="E123">
+        <v>90</v>
+      </c>
+      <c r="F123">
+        <v>62</v>
+      </c>
+      <c r="L123" t="s">
+        <v>157</v>
+      </c>
+      <c r="M123" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>187</v>
+      </c>
+      <c r="B124" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" t="s">
+        <v>32</v>
+      </c>
+      <c r="D124">
+        <v>6</v>
+      </c>
+      <c r="E124">
+        <v>78</v>
+      </c>
+      <c r="F124">
+        <v>59</v>
+      </c>
+      <c r="G124">
+        <v>97</v>
+      </c>
+      <c r="H124">
+        <v>46</v>
+      </c>
+      <c r="I124" t="s">
+        <v>159</v>
+      </c>
+      <c r="J124" t="s">
+        <v>27</v>
+      </c>
+      <c r="K124" t="s">
+        <v>28</v>
+      </c>
+      <c r="L124" t="s">
+        <v>157</v>
+      </c>
+      <c r="M124" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>188</v>
+      </c>
+      <c r="B125" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" t="s">
+        <v>29</v>
+      </c>
+      <c r="D125">
+        <v>6</v>
+      </c>
+      <c r="E125">
+        <v>97</v>
+      </c>
+      <c r="F125">
+        <v>46</v>
+      </c>
+      <c r="L125" t="s">
+        <v>159</v>
+      </c>
+      <c r="M125" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>189</v>
+      </c>
+      <c r="B126" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" t="s">
+        <v>32</v>
+      </c>
+      <c r="D126">
+        <v>6</v>
+      </c>
+      <c r="E126">
+        <v>97</v>
+      </c>
+      <c r="F126">
+        <v>44</v>
+      </c>
+      <c r="G126">
+        <v>84</v>
+      </c>
+      <c r="H126">
+        <v>4</v>
+      </c>
+      <c r="I126" t="s">
+        <v>91</v>
+      </c>
+      <c r="J126" t="s">
+        <v>27</v>
+      </c>
+      <c r="K126" t="s">
+        <v>28</v>
+      </c>
+      <c r="L126" t="s">
+        <v>159</v>
+      </c>
+      <c r="M126" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>190</v>
+      </c>
+      <c r="B127" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" t="s">
+        <v>29</v>
+      </c>
+      <c r="D127">
+        <v>6</v>
+      </c>
+      <c r="E127">
+        <v>84</v>
+      </c>
+      <c r="F127">
+        <v>5</v>
+      </c>
+      <c r="L127" t="s">
+        <v>91</v>
+      </c>
+      <c r="M127" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>191</v>
+      </c>
+      <c r="B128" t="s">
+        <v>15</v>
+      </c>
+      <c r="C128" t="s">
+        <v>32</v>
+      </c>
+      <c r="D128">
+        <v>6</v>
+      </c>
+      <c r="E128">
+        <v>80</v>
+      </c>
+      <c r="F128">
+        <v>4</v>
+      </c>
+      <c r="G128">
+        <v>64</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="I128" t="s">
+        <v>70</v>
+      </c>
+      <c r="J128" t="s">
+        <v>27</v>
+      </c>
+      <c r="K128" t="s">
+        <v>28</v>
+      </c>
+      <c r="L128" t="s">
+        <v>91</v>
+      </c>
+      <c r="M128" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>192</v>
+      </c>
+      <c r="B129" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" t="s">
+        <v>29</v>
+      </c>
+      <c r="D129">
+        <v>6</v>
+      </c>
+      <c r="E129">
+        <v>64</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="L129" t="s">
+        <v>70</v>
+      </c>
+      <c r="M129" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>193</v>
+      </c>
+      <c r="B130" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" t="s">
+        <v>32</v>
+      </c>
+      <c r="D130">
+        <v>6</v>
+      </c>
+      <c r="E130">
+        <v>68</v>
+      </c>
+      <c r="F130">
+        <v>6</v>
+      </c>
+      <c r="G130">
+        <v>93</v>
+      </c>
+      <c r="H130">
+        <v>18</v>
+      </c>
+      <c r="I130" t="s">
+        <v>45</v>
+      </c>
+      <c r="J130" t="s">
+        <v>27</v>
+      </c>
+      <c r="K130" t="s">
+        <v>28</v>
+      </c>
+      <c r="L130" t="s">
+        <v>70</v>
+      </c>
+      <c r="M130" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>194</v>
+      </c>
+      <c r="B131" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" t="s">
+        <v>29</v>
+      </c>
+      <c r="D131">
+        <v>6</v>
+      </c>
+      <c r="E131">
+        <v>93</v>
+      </c>
+      <c r="F131">
+        <v>18</v>
+      </c>
+      <c r="L131" t="s">
+        <v>45</v>
+      </c>
+      <c r="M131" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>195</v>
+      </c>
+      <c r="B132" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" t="s">
+        <v>32</v>
+      </c>
+      <c r="D132">
+        <v>6</v>
+      </c>
+      <c r="E132">
+        <v>94</v>
+      </c>
+      <c r="F132">
+        <v>18</v>
+      </c>
+      <c r="G132">
+        <v>87</v>
+      </c>
+      <c r="H132">
+        <v>62</v>
+      </c>
+      <c r="I132" t="s">
+        <v>157</v>
+      </c>
+      <c r="J132" t="s">
+        <v>27</v>
+      </c>
+      <c r="K132" t="s">
+        <v>28</v>
+      </c>
+      <c r="L132" t="s">
+        <v>45</v>
+      </c>
+      <c r="M132" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>196</v>
+      </c>
+      <c r="B133" t="s">
+        <v>15</v>
+      </c>
+      <c r="C133" t="s">
+        <v>29</v>
+      </c>
+      <c r="D133">
+        <v>6</v>
+      </c>
+      <c r="E133">
+        <v>87</v>
+      </c>
+      <c r="F133">
+        <v>62</v>
+      </c>
+      <c r="L133" t="s">
+        <v>157</v>
+      </c>
+      <c r="M133" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>197</v>
+      </c>
+      <c r="B134" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" t="s">
+        <v>32</v>
+      </c>
+      <c r="D134">
+        <v>6</v>
+      </c>
+      <c r="E134">
+        <v>70</v>
+      </c>
+      <c r="F134">
+        <v>58</v>
+      </c>
+      <c r="G134">
+        <v>47</v>
+      </c>
+      <c r="H134">
+        <v>80</v>
+      </c>
+      <c r="J134" t="s">
+        <v>58</v>
+      </c>
+      <c r="K134" t="s">
+        <v>33</v>
+      </c>
+      <c r="L134" t="s">
+        <v>157</v>
+      </c>
+      <c r="M134" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>198</v>
+      </c>
+      <c r="B135" t="s">
+        <v>14</v>
+      </c>
+      <c r="C135" t="s">
+        <v>53</v>
+      </c>
+      <c r="D135">
+        <v>6</v>
+      </c>
+      <c r="E135">
+        <v>47</v>
+      </c>
+      <c r="F135">
+        <v>80</v>
+      </c>
+      <c r="M135" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>199</v>
+      </c>
+      <c r="B136" t="s">
+        <v>14</v>
+      </c>
+      <c r="C136" t="s">
+        <v>32</v>
+      </c>
+      <c r="D136">
+        <v>7</v>
+      </c>
+      <c r="E136">
+        <v>47</v>
+      </c>
+      <c r="F136">
+        <v>80</v>
+      </c>
+      <c r="G136">
+        <v>67</v>
+      </c>
+      <c r="H136">
+        <v>78</v>
+      </c>
+      <c r="I136" t="s">
+        <v>26</v>
+      </c>
+      <c r="J136" t="s">
+        <v>27</v>
+      </c>
+      <c r="K136" t="s">
+        <v>33</v>
+      </c>
+      <c r="L136" t="s">
+        <v>60</v>
+      </c>
+      <c r="M136" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>200</v>
+      </c>
+      <c r="B137" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137" t="s">
+        <v>32</v>
+      </c>
+      <c r="D137">
+        <v>7</v>
+      </c>
+      <c r="E137">
+        <v>67</v>
+      </c>
+      <c r="F137">
+        <v>78</v>
+      </c>
+      <c r="G137">
+        <v>72</v>
+      </c>
+      <c r="H137">
+        <v>76</v>
+      </c>
+      <c r="J137" t="s">
+        <v>58</v>
+      </c>
+      <c r="K137" t="s">
+        <v>33</v>
+      </c>
+      <c r="L137" t="s">
+        <v>26</v>
+      </c>
+      <c r="M137" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>201</v>
+      </c>
+      <c r="B138" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" t="s">
+        <v>32</v>
+      </c>
+      <c r="D138">
+        <v>7</v>
+      </c>
+      <c r="E138">
+        <v>72</v>
+      </c>
+      <c r="F138">
+        <v>76</v>
+      </c>
+      <c r="G138">
+        <v>70</v>
+      </c>
+      <c r="H138">
+        <v>63</v>
+      </c>
+      <c r="I138" t="s">
+        <v>56</v>
+      </c>
+      <c r="J138" t="s">
+        <v>27</v>
+      </c>
+      <c r="K138" t="s">
+        <v>36</v>
+      </c>
+      <c r="L138" t="s">
+        <v>157</v>
+      </c>
+      <c r="M138" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>202</v>
+      </c>
+      <c r="B139" t="s">
+        <v>15</v>
+      </c>
+      <c r="C139" t="s">
+        <v>29</v>
+      </c>
+      <c r="D139">
+        <v>7</v>
+      </c>
+      <c r="E139">
+        <v>70</v>
+      </c>
+      <c r="F139">
+        <v>63</v>
+      </c>
+      <c r="L139" t="s">
+        <v>56</v>
+      </c>
+      <c r="M139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>203</v>
+      </c>
+      <c r="B140" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" t="s">
+        <v>32</v>
+      </c>
+      <c r="D140">
+        <v>7</v>
+      </c>
+      <c r="E140">
+        <v>68</v>
+      </c>
+      <c r="F140">
+        <v>57</v>
+      </c>
+      <c r="G140">
+        <v>61</v>
+      </c>
+      <c r="H140">
+        <v>42</v>
+      </c>
+      <c r="I140" t="s">
+        <v>70</v>
+      </c>
+      <c r="J140" t="s">
+        <v>27</v>
+      </c>
+      <c r="K140" t="s">
+        <v>28</v>
+      </c>
+      <c r="L140" t="s">
+        <v>56</v>
+      </c>
+      <c r="M140" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>204</v>
+      </c>
+      <c r="B141" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" t="s">
+        <v>29</v>
+      </c>
+      <c r="D141">
+        <v>7</v>
+      </c>
+      <c r="E141">
+        <v>61</v>
+      </c>
+      <c r="F141">
+        <v>42</v>
+      </c>
+      <c r="L141" t="s">
+        <v>70</v>
+      </c>
+      <c r="M141" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>205</v>
+      </c>
+      <c r="B142" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" t="s">
+        <v>97</v>
+      </c>
+      <c r="D142">
+        <v>7</v>
+      </c>
+      <c r="E142">
+        <v>60</v>
+      </c>
+      <c r="F142">
+        <v>50</v>
+      </c>
+      <c r="L142" t="s">
+        <v>70</v>
+      </c>
+      <c r="M142" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>206</v>
+      </c>
+      <c r="B143" t="s">
+        <v>15</v>
+      </c>
+      <c r="C143" t="s">
+        <v>32</v>
+      </c>
+      <c r="D143">
+        <v>7</v>
+      </c>
+      <c r="E143">
+        <v>46</v>
+      </c>
+      <c r="F143">
+        <v>52</v>
+      </c>
+      <c r="G143">
+        <v>16</v>
+      </c>
+      <c r="H143">
+        <v>78</v>
+      </c>
+      <c r="I143" t="s">
+        <v>55</v>
+      </c>
+      <c r="J143" t="s">
+        <v>27</v>
+      </c>
+      <c r="K143" t="s">
+        <v>28</v>
+      </c>
+      <c r="L143" t="s">
+        <v>70</v>
+      </c>
+      <c r="M143" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>207</v>
+      </c>
+      <c r="B144" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" t="s">
+        <v>29</v>
+      </c>
+      <c r="D144">
+        <v>7</v>
+      </c>
+      <c r="E144">
+        <v>16</v>
+      </c>
+      <c r="F144">
+        <v>78</v>
+      </c>
+      <c r="L144" t="s">
+        <v>55</v>
+      </c>
+      <c r="M144" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>208</v>
+      </c>
+      <c r="B145" t="s">
+        <v>15</v>
+      </c>
+      <c r="C145" t="s">
+        <v>32</v>
+      </c>
+      <c r="D145">
+        <v>7</v>
+      </c>
+      <c r="E145">
+        <v>7</v>
+      </c>
+      <c r="F145">
+        <v>78</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+      <c r="H145">
+        <v>44</v>
+      </c>
+      <c r="J145" t="s">
+        <v>58</v>
+      </c>
+      <c r="K145" t="s">
+        <v>36</v>
+      </c>
+      <c r="L145" t="s">
+        <v>55</v>
+      </c>
+      <c r="M145" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>209</v>
+      </c>
+      <c r="B146" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146" t="s">
+        <v>114</v>
+      </c>
+      <c r="D146">
+        <v>7</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>44</v>
+      </c>
+      <c r="L146" t="s">
+        <v>115</v>
+      </c>
+      <c r="M146" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>210</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147">
+        <v>7</v>
+      </c>
+      <c r="E147">
+        <v>16</v>
+      </c>
+      <c r="F147">
+        <v>40</v>
+      </c>
+      <c r="G147">
+        <v>74</v>
+      </c>
+      <c r="H147">
+        <v>18</v>
+      </c>
+      <c r="I147" t="s">
+        <v>40</v>
+      </c>
+      <c r="J147" t="s">
+        <v>27</v>
+      </c>
+      <c r="K147" t="s">
+        <v>33</v>
+      </c>
+      <c r="L147" t="s">
+        <v>115</v>
+      </c>
+      <c r="M147" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>211</v>
+      </c>
+      <c r="B148" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148" t="s">
+        <v>29</v>
+      </c>
+      <c r="D148">
+        <v>7</v>
+      </c>
+      <c r="E148">
+        <v>74</v>
+      </c>
+      <c r="F148">
+        <v>18</v>
+      </c>
+      <c r="L148" t="s">
+        <v>40</v>
+      </c>
+      <c r="M148" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>212</v>
+      </c>
+      <c r="B149" t="s">
+        <v>14</v>
+      </c>
+      <c r="C149" t="s">
+        <v>32</v>
+      </c>
+      <c r="D149">
+        <v>7</v>
+      </c>
+      <c r="E149">
+        <v>72</v>
+      </c>
+      <c r="F149">
+        <v>14</v>
+      </c>
+      <c r="G149">
+        <v>66</v>
+      </c>
+      <c r="H149">
+        <v>3</v>
+      </c>
+      <c r="I149" t="s">
+        <v>124</v>
+      </c>
+      <c r="J149" t="s">
+        <v>27</v>
+      </c>
+      <c r="K149" t="s">
+        <v>28</v>
+      </c>
+      <c r="L149" t="s">
+        <v>40</v>
+      </c>
+      <c r="M149" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>213</v>
+      </c>
+      <c r="B150" t="s">
+        <v>14</v>
+      </c>
+      <c r="C150" t="s">
+        <v>29</v>
+      </c>
+      <c r="D150">
+        <v>7</v>
+      </c>
+      <c r="E150">
+        <v>66</v>
+      </c>
+      <c r="F150">
+        <v>3</v>
+      </c>
+      <c r="L150" t="s">
+        <v>124</v>
+      </c>
+      <c r="M150" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>214</v>
+      </c>
+      <c r="B151" t="s">
+        <v>14</v>
+      </c>
+      <c r="C151" t="s">
+        <v>32</v>
+      </c>
+      <c r="D151">
+        <v>7</v>
+      </c>
+      <c r="E151">
+        <v>66</v>
+      </c>
+      <c r="F151">
+        <v>3</v>
+      </c>
+      <c r="G151">
+        <v>64</v>
+      </c>
+      <c r="H151">
+        <v>17</v>
+      </c>
+      <c r="I151" t="s">
+        <v>87</v>
+      </c>
+      <c r="J151" t="s">
+        <v>27</v>
+      </c>
+      <c r="K151" t="s">
+        <v>28</v>
+      </c>
+      <c r="L151" t="s">
+        <v>124</v>
+      </c>
+      <c r="M151" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>215</v>
+      </c>
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" t="s">
+        <v>32</v>
+      </c>
+      <c r="D152">
+        <v>7</v>
+      </c>
+      <c r="E152">
+        <v>64</v>
+      </c>
+      <c r="F152">
+        <v>17</v>
+      </c>
+      <c r="G152">
+        <v>61</v>
+      </c>
+      <c r="H152">
+        <v>2</v>
+      </c>
+      <c r="I152" t="s">
+        <v>105</v>
+      </c>
+      <c r="J152" t="s">
+        <v>27</v>
+      </c>
+      <c r="K152" t="s">
+        <v>28</v>
+      </c>
+      <c r="L152" t="s">
+        <v>87</v>
+      </c>
+      <c r="M152" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>216</v>
+      </c>
+      <c r="B153" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153" t="s">
+        <v>32</v>
+      </c>
+      <c r="D153">
+        <v>7</v>
+      </c>
+      <c r="E153">
+        <v>61</v>
+      </c>
+      <c r="F153">
+        <v>2</v>
+      </c>
+      <c r="G153">
+        <v>68</v>
+      </c>
+      <c r="H153">
+        <v>2</v>
+      </c>
+      <c r="I153" t="s">
+        <v>124</v>
+      </c>
+      <c r="J153" t="s">
+        <v>27</v>
+      </c>
+      <c r="K153" t="s">
+        <v>28</v>
+      </c>
+      <c r="L153" t="s">
+        <v>105</v>
+      </c>
+      <c r="M153" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>217</v>
+      </c>
+      <c r="B154" t="s">
+        <v>14</v>
+      </c>
+      <c r="C154" t="s">
+        <v>29</v>
+      </c>
+      <c r="D154">
+        <v>7</v>
+      </c>
+      <c r="E154">
+        <v>68</v>
+      </c>
+      <c r="F154">
+        <v>2</v>
+      </c>
+      <c r="L154" t="s">
+        <v>124</v>
+      </c>
+      <c r="M154" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>218</v>
+      </c>
+      <c r="B155" t="s">
+        <v>14</v>
+      </c>
+      <c r="C155" t="s">
+        <v>154</v>
+      </c>
+      <c r="D155">
+        <v>7</v>
+      </c>
+      <c r="E155">
+        <v>66</v>
+      </c>
+      <c r="F155">
+        <v>2</v>
+      </c>
+      <c r="L155" t="s">
+        <v>124</v>
+      </c>
+      <c r="M155" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>219</v>
+      </c>
+      <c r="B156" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" t="s">
+        <v>78</v>
+      </c>
+      <c r="D156">
+        <v>7</v>
+      </c>
+      <c r="E156">
+        <v>66</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="L156" t="s">
+        <v>70</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>220</v>
+      </c>
+      <c r="B157" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157" t="s">
+        <v>32</v>
+      </c>
+      <c r="D157">
+        <v>8</v>
+      </c>
+      <c r="E157">
+        <v>66</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+      <c r="G157">
+        <v>48</v>
+      </c>
+      <c r="H157">
+        <v>19</v>
+      </c>
+      <c r="I157" t="s">
+        <v>25</v>
+      </c>
+      <c r="J157" t="s">
+        <v>27</v>
+      </c>
+      <c r="K157" t="s">
+        <v>28</v>
+      </c>
+      <c r="L157" t="s">
+        <v>105</v>
+      </c>
+      <c r="M157" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>221</v>
+      </c>
+      <c r="B158" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158" t="s">
+        <v>32</v>
+      </c>
+      <c r="D158">
+        <v>8</v>
+      </c>
+      <c r="E158">
+        <v>48</v>
+      </c>
+      <c r="F158">
+        <v>19</v>
+      </c>
+      <c r="G158">
+        <v>51</v>
+      </c>
+      <c r="H158">
+        <v>52</v>
+      </c>
+      <c r="I158" t="s">
+        <v>51</v>
+      </c>
+      <c r="J158" t="s">
+        <v>27</v>
+      </c>
+      <c r="K158" t="s">
+        <v>28</v>
+      </c>
+      <c r="L158" t="s">
+        <v>25</v>
+      </c>
+      <c r="M158" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>222</v>
+      </c>
+      <c r="B159" t="s">
+        <v>14</v>
+      </c>
+      <c r="C159" t="s">
+        <v>29</v>
+      </c>
+      <c r="D159">
+        <v>8</v>
+      </c>
+      <c r="E159">
+        <v>51</v>
+      </c>
+      <c r="F159">
+        <v>52</v>
+      </c>
+      <c r="L159" t="s">
+        <v>51</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>223</v>
+      </c>
+      <c r="B160" t="s">
+        <v>14</v>
+      </c>
+      <c r="C160" t="s">
+        <v>32</v>
+      </c>
+      <c r="D160">
+        <v>8</v>
+      </c>
+      <c r="E160">
+        <v>60</v>
+      </c>
+      <c r="F160">
+        <v>62</v>
+      </c>
+      <c r="G160">
+        <v>69</v>
+      </c>
+      <c r="H160">
+        <v>79</v>
+      </c>
+      <c r="I160" t="s">
+        <v>60</v>
+      </c>
+      <c r="J160" t="s">
+        <v>27</v>
+      </c>
+      <c r="K160" t="s">
+        <v>28</v>
+      </c>
+      <c r="L160" t="s">
+        <v>51</v>
+      </c>
+      <c r="M160" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>225</v>
+      </c>
+      <c r="B161" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161" t="s">
+        <v>29</v>
+      </c>
+      <c r="D161">
+        <v>8</v>
+      </c>
+      <c r="E161">
+        <v>69</v>
+      </c>
+      <c r="F161">
+        <v>79</v>
+      </c>
+      <c r="L161" t="s">
+        <v>60</v>
+      </c>
+      <c r="M161" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>224</v>
+      </c>
+      <c r="B162" t="s">
+        <v>14</v>
+      </c>
+      <c r="C162" t="s">
+        <v>32</v>
+      </c>
+      <c r="D162">
+        <v>8</v>
+      </c>
+      <c r="E162">
+        <v>69</v>
+      </c>
+      <c r="F162">
+        <v>79</v>
+      </c>
+      <c r="G162">
+        <v>49</v>
+      </c>
+      <c r="H162">
+        <v>74</v>
+      </c>
+      <c r="I162" t="s">
+        <v>51</v>
+      </c>
+      <c r="J162" t="s">
+        <v>27</v>
+      </c>
+      <c r="K162" t="s">
+        <v>28</v>
+      </c>
+      <c r="L162" t="s">
+        <v>60</v>
+      </c>
+      <c r="M162" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>226</v>
+      </c>
+      <c r="B163" t="s">
+        <v>14</v>
+      </c>
+      <c r="C163" t="s">
+        <v>32</v>
+      </c>
+      <c r="D163">
+        <v>8</v>
+      </c>
+      <c r="E163">
+        <v>49</v>
+      </c>
+      <c r="F163">
+        <v>74</v>
+      </c>
+      <c r="G163">
+        <v>22</v>
+      </c>
+      <c r="H163">
+        <v>46</v>
+      </c>
+      <c r="I163" t="s">
+        <v>115</v>
+      </c>
+      <c r="J163" t="s">
+        <v>27</v>
+      </c>
+      <c r="K163" t="s">
+        <v>28</v>
+      </c>
+      <c r="L163" t="s">
+        <v>51</v>
+      </c>
+      <c r="M163" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>227</v>
+      </c>
+      <c r="B164" t="s">
+        <v>14</v>
+      </c>
+      <c r="C164" t="s">
+        <v>32</v>
+      </c>
+      <c r="D164">
+        <v>8</v>
+      </c>
+      <c r="E164">
+        <v>22</v>
+      </c>
+      <c r="F164">
+        <v>46</v>
+      </c>
+      <c r="G164">
+        <v>28</v>
+      </c>
+      <c r="H164">
+        <v>25</v>
+      </c>
+      <c r="I164" t="s">
+        <v>25</v>
+      </c>
+      <c r="J164" t="s">
+        <v>27</v>
+      </c>
+      <c r="K164" t="s">
+        <v>28</v>
+      </c>
+      <c r="L164" t="s">
+        <v>115</v>
+      </c>
+      <c r="M164" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>228</v>
+      </c>
+      <c r="B165" t="s">
+        <v>14</v>
+      </c>
+      <c r="C165" t="s">
+        <v>29</v>
+      </c>
+      <c r="D165">
+        <v>8</v>
+      </c>
+      <c r="E165">
+        <v>28</v>
+      </c>
+      <c r="F165">
+        <v>25</v>
+      </c>
+      <c r="L165" t="s">
+        <v>25</v>
+      </c>
+      <c r="M165" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>229</v>
+      </c>
+      <c r="B166" t="s">
+        <v>14</v>
+      </c>
+      <c r="C166" t="s">
+        <v>32</v>
+      </c>
+      <c r="D166">
+        <v>8</v>
+      </c>
+      <c r="E166">
+        <v>34</v>
+      </c>
+      <c r="F166">
+        <v>23</v>
+      </c>
+      <c r="G166">
+        <v>67</v>
+      </c>
+      <c r="H166">
+        <v>52</v>
+      </c>
+      <c r="I166" t="s">
+        <v>26</v>
+      </c>
+      <c r="J166" t="s">
+        <v>27</v>
+      </c>
+      <c r="K166" t="s">
+        <v>33</v>
+      </c>
+      <c r="L166" t="s">
+        <v>25</v>
+      </c>
+      <c r="M166" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>230</v>
+      </c>
+      <c r="B167" t="s">
+        <v>14</v>
+      </c>
+      <c r="C167" t="s">
+        <v>32</v>
+      </c>
+      <c r="D167">
+        <v>8</v>
+      </c>
+      <c r="E167">
+        <v>67</v>
+      </c>
+      <c r="F167">
+        <v>52</v>
+      </c>
+      <c r="G167">
+        <v>74</v>
+      </c>
+      <c r="H167">
+        <v>68</v>
+      </c>
+      <c r="I167" t="s">
+        <v>60</v>
+      </c>
+      <c r="J167" t="s">
+        <v>27</v>
+      </c>
+      <c r="K167" t="s">
+        <v>36</v>
+      </c>
+      <c r="L167" t="s">
+        <v>26</v>
+      </c>
+      <c r="M167" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>231</v>
+      </c>
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168">
+        <v>8</v>
+      </c>
+      <c r="E168">
+        <v>74</v>
+      </c>
+      <c r="F168">
+        <v>68</v>
+      </c>
+      <c r="L168" t="s">
+        <v>60</v>
+      </c>
+      <c r="M168" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>232</v>
+      </c>
+      <c r="B169" t="s">
+        <v>14</v>
+      </c>
+      <c r="C169" t="s">
+        <v>32</v>
+      </c>
+      <c r="D169">
+        <v>8</v>
+      </c>
+      <c r="E169">
+        <v>87</v>
+      </c>
+      <c r="F169">
+        <v>60</v>
+      </c>
+      <c r="G169">
+        <v>105</v>
+      </c>
+      <c r="H169">
+        <v>32</v>
+      </c>
+      <c r="J169" t="s">
+        <v>58</v>
+      </c>
+      <c r="K169" t="s">
+        <v>33</v>
+      </c>
+      <c r="L169" t="s">
+        <v>60</v>
+      </c>
+      <c r="M169" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>233</v>
+      </c>
+      <c r="B170" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" t="s">
+        <v>43</v>
+      </c>
+      <c r="D170">
+        <v>8</v>
+      </c>
+      <c r="E170">
+        <v>105</v>
+      </c>
+      <c r="F170">
+        <v>32</v>
+      </c>
+      <c r="G170">
+        <v>86</v>
+      </c>
+      <c r="H170">
+        <v>24</v>
+      </c>
+      <c r="L170" t="s">
+        <v>45</v>
+      </c>
+      <c r="M170" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>234</v>
+      </c>
+      <c r="B171" t="s">
+        <v>15</v>
+      </c>
+      <c r="C171" t="s">
+        <v>32</v>
+      </c>
+      <c r="D171">
+        <v>8</v>
+      </c>
+      <c r="E171">
+        <v>86</v>
+      </c>
+      <c r="F171">
+        <v>24</v>
+      </c>
+      <c r="G171">
+        <v>63</v>
+      </c>
+      <c r="H171">
+        <v>32</v>
+      </c>
+      <c r="J171" t="s">
+        <v>58</v>
+      </c>
+      <c r="K171" t="s">
+        <v>33</v>
+      </c>
+      <c r="L171" t="s">
+        <v>70</v>
+      </c>
+      <c r="M171" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>235</v>
+      </c>
+      <c r="B172" t="s">
+        <v>14</v>
+      </c>
+      <c r="C172" t="s">
+        <v>29</v>
+      </c>
+      <c r="D172">
+        <v>8</v>
+      </c>
+      <c r="E172">
+        <v>63</v>
+      </c>
+      <c r="F172">
+        <v>32</v>
+      </c>
+      <c r="L172" t="s">
+        <v>25</v>
+      </c>
+      <c r="M172" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
[Actualizamos la base de datos] Victor
</commit_message>
<xml_diff>
--- a/eventos.xlsx
+++ b/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Víctor\Desktop\IronHack\Apuntes\Futbol_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE067536-40C5-4390-B8D4-598046C9413D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41027F7-355B-4FA8-B6BF-DDBBA8F032BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="245">
   <si>
     <t>timestamp</t>
   </si>
@@ -733,6 +733,33 @@
   </si>
   <si>
     <t>00:08:37.820</t>
+  </si>
+  <si>
+    <t>00:08:39.820</t>
+  </si>
+  <si>
+    <t>00:08:40.820</t>
+  </si>
+  <si>
+    <t>00:08:41.820</t>
+  </si>
+  <si>
+    <t>00:08:42.820</t>
+  </si>
+  <si>
+    <t>00:08:47.820</t>
+  </si>
+  <si>
+    <t>00:08:51.820</t>
+  </si>
+  <si>
+    <t>00:08:56.820</t>
+  </si>
+  <si>
+    <t>00:09:00.820</t>
+  </si>
+  <si>
+    <t>00:09:02.820</t>
   </si>
 </sst>
 </file>
@@ -775,10 +802,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T172"/>
+  <dimension ref="A1:T181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6007,7 +6033,7 @@
       <c r="L151" t="s">
         <v>124</v>
       </c>
-      <c r="M151" s="2" t="s">
+      <c r="M151" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6048,7 +6074,7 @@
       <c r="L152" t="s">
         <v>87</v>
       </c>
-      <c r="M152" s="2" t="s">
+      <c r="M152" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6089,7 +6115,7 @@
       <c r="L153" t="s">
         <v>105</v>
       </c>
-      <c r="M153" s="2" t="s">
+      <c r="M153" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6115,7 +6141,7 @@
       <c r="L154" t="s">
         <v>124</v>
       </c>
-      <c r="M154" s="2" t="s">
+      <c r="M154" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6141,7 +6167,7 @@
       <c r="L155" t="s">
         <v>124</v>
       </c>
-      <c r="M155" s="2" t="s">
+      <c r="M155" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6167,7 +6193,7 @@
       <c r="L156" t="s">
         <v>70</v>
       </c>
-      <c r="M156" s="2" t="s">
+      <c r="M156" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6208,7 +6234,7 @@
       <c r="L157" t="s">
         <v>105</v>
       </c>
-      <c r="M157" s="2" t="s">
+      <c r="M157" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6249,7 +6275,7 @@
       <c r="L158" t="s">
         <v>25</v>
       </c>
-      <c r="M158" s="2" t="s">
+      <c r="M158" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6275,7 +6301,7 @@
       <c r="L159" t="s">
         <v>51</v>
       </c>
-      <c r="M159" s="2" t="s">
+      <c r="M159" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6316,7 +6342,7 @@
       <c r="L160" t="s">
         <v>51</v>
       </c>
-      <c r="M160" s="2" t="s">
+      <c r="M160" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6342,7 +6368,7 @@
       <c r="L161" t="s">
         <v>60</v>
       </c>
-      <c r="M161" s="2" t="s">
+      <c r="M161" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6383,7 +6409,7 @@
       <c r="L162" t="s">
         <v>60</v>
       </c>
-      <c r="M162" s="2" t="s">
+      <c r="M162" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6424,7 +6450,7 @@
       <c r="L163" t="s">
         <v>51</v>
       </c>
-      <c r="M163" s="2" t="s">
+      <c r="M163" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6465,7 +6491,7 @@
       <c r="L164" t="s">
         <v>115</v>
       </c>
-      <c r="M164" s="2" t="s">
+      <c r="M164" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6491,7 +6517,7 @@
       <c r="L165" t="s">
         <v>25</v>
       </c>
-      <c r="M165" s="2" t="s">
+      <c r="M165" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6532,7 +6558,7 @@
       <c r="L166" t="s">
         <v>25</v>
       </c>
-      <c r="M166" s="2" t="s">
+      <c r="M166" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6573,7 +6599,7 @@
       <c r="L167" t="s">
         <v>26</v>
       </c>
-      <c r="M167" s="2" t="s">
+      <c r="M167" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6599,7 +6625,7 @@
       <c r="L168" t="s">
         <v>60</v>
       </c>
-      <c r="M168" s="2" t="s">
+      <c r="M168" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6637,7 +6663,7 @@
       <c r="L169" t="s">
         <v>60</v>
       </c>
-      <c r="M169" s="2" t="s">
+      <c r="M169" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6669,7 +6695,7 @@
       <c r="L170" t="s">
         <v>45</v>
       </c>
-      <c r="M170" s="2" t="s">
+      <c r="M170" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6733,8 +6759,344 @@
       <c r="L172" t="s">
         <v>25</v>
       </c>
-      <c r="M172" s="2" t="s">
-        <v>14</v>
+      <c r="M172" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>236</v>
+      </c>
+      <c r="B173" t="s">
+        <v>14</v>
+      </c>
+      <c r="C173" t="s">
+        <v>32</v>
+      </c>
+      <c r="D173">
+        <v>8</v>
+      </c>
+      <c r="E173">
+        <v>68</v>
+      </c>
+      <c r="F173">
+        <v>25</v>
+      </c>
+      <c r="G173">
+        <v>84</v>
+      </c>
+      <c r="H173">
+        <v>32</v>
+      </c>
+      <c r="J173" t="s">
+        <v>58</v>
+      </c>
+      <c r="K173" t="s">
+        <v>28</v>
+      </c>
+      <c r="L173" t="s">
+        <v>25</v>
+      </c>
+      <c r="M173" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>237</v>
+      </c>
+      <c r="B174" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" t="s">
+        <v>66</v>
+      </c>
+      <c r="D174">
+        <v>8</v>
+      </c>
+      <c r="E174">
+        <v>84</v>
+      </c>
+      <c r="F174">
+        <v>32</v>
+      </c>
+      <c r="L174" t="s">
+        <v>56</v>
+      </c>
+      <c r="M174" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>238</v>
+      </c>
+      <c r="B175" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" t="s">
+        <v>29</v>
+      </c>
+      <c r="D175">
+        <v>8</v>
+      </c>
+      <c r="E175">
+        <v>84</v>
+      </c>
+      <c r="F175">
+        <v>42</v>
+      </c>
+      <c r="L175" t="s">
+        <v>77</v>
+      </c>
+      <c r="M175" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>239</v>
+      </c>
+      <c r="B176" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" t="s">
+        <v>32</v>
+      </c>
+      <c r="D176">
+        <v>8</v>
+      </c>
+      <c r="E176">
+        <v>84</v>
+      </c>
+      <c r="F176">
+        <v>42</v>
+      </c>
+      <c r="G176">
+        <v>74</v>
+      </c>
+      <c r="H176">
+        <v>61</v>
+      </c>
+      <c r="I176" t="s">
+        <v>55</v>
+      </c>
+      <c r="J176" t="s">
+        <v>27</v>
+      </c>
+      <c r="K176" t="s">
+        <v>28</v>
+      </c>
+      <c r="L176" t="s">
+        <v>77</v>
+      </c>
+      <c r="M176" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>240</v>
+      </c>
+      <c r="B177" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" t="s">
+        <v>32</v>
+      </c>
+      <c r="D177">
+        <v>8</v>
+      </c>
+      <c r="E177">
+        <v>62</v>
+      </c>
+      <c r="F177">
+        <v>70</v>
+      </c>
+      <c r="G177">
+        <v>76</v>
+      </c>
+      <c r="H177">
+        <v>60</v>
+      </c>
+      <c r="I177" t="s">
+        <v>157</v>
+      </c>
+      <c r="J177" t="s">
+        <v>27</v>
+      </c>
+      <c r="K177" t="s">
+        <v>33</v>
+      </c>
+      <c r="L177" t="s">
+        <v>55</v>
+      </c>
+      <c r="M177" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>241</v>
+      </c>
+      <c r="B178" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" t="s">
+        <v>32</v>
+      </c>
+      <c r="D178">
+        <v>8</v>
+      </c>
+      <c r="E178">
+        <v>76</v>
+      </c>
+      <c r="F178">
+        <v>60</v>
+      </c>
+      <c r="G178">
+        <v>95</v>
+      </c>
+      <c r="H178">
+        <v>30</v>
+      </c>
+      <c r="I178" t="s">
+        <v>45</v>
+      </c>
+      <c r="J178" t="s">
+        <v>27</v>
+      </c>
+      <c r="K178" t="s">
+        <v>28</v>
+      </c>
+      <c r="L178" t="s">
+        <v>157</v>
+      </c>
+      <c r="M178" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>242</v>
+      </c>
+      <c r="B179" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" t="s">
+        <v>32</v>
+      </c>
+      <c r="D179">
+        <v>8</v>
+      </c>
+      <c r="E179">
+        <v>81</v>
+      </c>
+      <c r="F179">
+        <v>18</v>
+      </c>
+      <c r="G179">
+        <v>65</v>
+      </c>
+      <c r="H179">
+        <v>3</v>
+      </c>
+      <c r="I179" t="s">
+        <v>91</v>
+      </c>
+      <c r="J179" t="s">
+        <v>27</v>
+      </c>
+      <c r="K179" t="s">
+        <v>28</v>
+      </c>
+      <c r="L179" t="s">
+        <v>45</v>
+      </c>
+      <c r="M179" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>243</v>
+      </c>
+      <c r="B180" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180" t="s">
+        <v>32</v>
+      </c>
+      <c r="D180">
+        <v>9</v>
+      </c>
+      <c r="E180">
+        <v>65</v>
+      </c>
+      <c r="F180">
+        <v>3</v>
+      </c>
+      <c r="G180">
+        <v>53</v>
+      </c>
+      <c r="H180">
+        <v>9</v>
+      </c>
+      <c r="I180" t="s">
+        <v>48</v>
+      </c>
+      <c r="J180" t="s">
+        <v>27</v>
+      </c>
+      <c r="K180" t="s">
+        <v>28</v>
+      </c>
+      <c r="L180" t="s">
+        <v>91</v>
+      </c>
+      <c r="M180" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>244</v>
+      </c>
+      <c r="B181" t="s">
+        <v>15</v>
+      </c>
+      <c r="C181" t="s">
+        <v>32</v>
+      </c>
+      <c r="D181">
+        <v>9</v>
+      </c>
+      <c r="E181">
+        <v>52</v>
+      </c>
+      <c r="F181">
+        <v>8</v>
+      </c>
+      <c r="G181">
+        <v>50</v>
+      </c>
+      <c r="H181">
+        <v>2</v>
+      </c>
+      <c r="I181" t="s">
+        <v>70</v>
+      </c>
+      <c r="J181" t="s">
+        <v>27</v>
+      </c>
+      <c r="K181" t="s">
+        <v>28</v>
+      </c>
+      <c r="L181" t="s">
+        <v>48</v>
+      </c>
+      <c r="M181" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>